<commit_message>
Running model versions 1-4
</commit_message>
<xml_diff>
--- a/SBTF_data/input_data/radio_tower_locations/RTEastNorth_8groups.xlsx
+++ b/SBTF_data/input_data/radio_tower_locations/RTEastNorth_8groups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\ml4rt\Example_data\Input\Radio_tower_locations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s5236256\Documents\GitHub\ml4rt\SBTF_data\input_data\radio_tower_locations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73E86FC-2DCC-4059-A8E8-4A707275454F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA513D65-1256-4CC6-A98C-A540A862E3EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{12628E73-B5DB-4716-98A2-AEE23607AF74}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12628E73-B5DB-4716-98A2-AEE23607AF74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>Type</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t>TowerID</t>
-  </si>
-  <si>
-    <t>RT28</t>
   </si>
   <si>
     <t>zone_number</t>
@@ -496,20 +493,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30D9363-B02E-4743-9288-10C65779E531}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -523,16 +520,16 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
       <c r="G1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -549,13 +546,13 @@
         <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -572,13 +569,13 @@
         <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -595,13 +592,13 @@
         <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -618,13 +615,13 @@
         <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -641,13 +638,13 @@
         <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -664,13 +661,13 @@
         <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -687,13 +684,13 @@
         <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -710,13 +707,13 @@
         <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -733,13 +730,13 @@
         <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -756,13 +753,13 @@
         <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -779,13 +776,13 @@
         <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -802,13 +799,13 @@
         <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -825,13 +822,13 @@
         <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -848,13 +845,13 @@
         <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -871,13 +868,13 @@
         <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -894,13 +891,13 @@
         <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -917,13 +914,13 @@
         <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -940,13 +937,13 @@
         <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -963,13 +960,13 @@
         <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -986,13 +983,13 @@
         <v>55</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1009,13 +1006,13 @@
         <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1032,13 +1029,13 @@
         <v>55</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1055,13 +1052,13 @@
         <v>55</v>
       </c>
       <c r="F24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1078,13 +1075,13 @@
         <v>55</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1101,13 +1098,13 @@
         <v>55</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1124,13 +1121,13 @@
         <v>55</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1147,33 +1144,10 @@
         <v>55</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>428298</v>
-      </c>
-      <c r="D29">
-        <v>7572855</v>
-      </c>
-      <c r="E29">
-        <v>55</v>
-      </c>
-      <c r="F29" t="s">
-        <v>35</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>